<commit_message>
mi primera pagina web
</commit_message>
<xml_diff>
--- a/DATOS DE PRACTICAS_INIA/FICHA DE EVALUACIÓN DE ADULTOS.xlsx
+++ b/DATOS DE PRACTICAS_INIA/FICHA DE EVALUACIÓN DE ADULTOS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\INGENIERIA AGRONOMA-LLEYNER\DATOS DE PRACTICAS-INIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LLEYNER\Documents\Roman-Peña\DATOS DE PRACTICAS_INIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C92B621-7D17-4EA0-B99C-05307C4A59ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A84E6F2-30E6-403C-92CC-4A7A37EEF9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{1705B625-BC10-4EF5-800C-BE114087651C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1705B625-BC10-4EF5-800C-BE114087651C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -674,7 +674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA972AA-047F-48A0-84CD-36172394DCE5}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
@@ -3369,7 +3369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F11FC8-0538-4C42-8D21-8E81F3CCA81B}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
@@ -4591,7 +4591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09FCC7D-7B57-4581-A91F-7FDC1FF210B0}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
@@ -7035,7 +7035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0B51DA-444E-4E0A-937C-04F190AF25AE}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
@@ -8260,8 +8260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3D435-86DD-4679-9BBB-DECA22DB302A}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N43"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8360,9 +8360,15 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>18</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -8382,9 +8388,15 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -8404,9 +8416,15 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>59</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -8426,9 +8444,15 @@
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1">
+        <v>13</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -8448,9 +8472,15 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>56</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -8470,9 +8500,15 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>64</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -8492,9 +8528,15 @@
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1">
+        <v>93</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -8514,9 +8556,15 @@
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>47</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -8536,9 +8584,15 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>9</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -8558,9 +8612,15 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>7</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -8580,9 +8640,15 @@
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>6</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -8602,9 +8668,15 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>4</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -8624,9 +8696,15 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>88</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -8646,9 +8724,15 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>96</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -8668,9 +8752,15 @@
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1">
+        <v>81</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -8690,9 +8780,15 @@
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="F19" s="1">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>48</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -8712,9 +8808,15 @@
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="F20" s="1">
+        <v>5</v>
+      </c>
+      <c r="G20" s="1">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1">
+        <v>69</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -8734,9 +8836,15 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>3</v>
+      </c>
+      <c r="H21" s="1">
+        <v>31</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -8756,9 +8864,15 @@
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>15</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -8778,9 +8892,15 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="F23" s="1">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>6</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -8800,9 +8920,15 @@
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>10</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -8822,9 +8948,15 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="F25" s="1">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>5</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -8844,9 +8976,15 @@
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>51</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -8866,9 +9004,15 @@
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>3</v>
+      </c>
+      <c r="H27" s="1">
+        <v>92</v>
+      </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -8888,9 +9032,15 @@
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1">
+        <v>35</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -8910,9 +9060,15 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1">
+        <v>41</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -8932,9 +9088,15 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>6</v>
+      </c>
+      <c r="H30" s="1">
+        <v>94</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -8954,9 +9116,15 @@
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1">
+        <v>26</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -8976,9 +9144,15 @@
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>17</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -8998,9 +9172,15 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="F33" s="1">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <v>6</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -9020,9 +9200,15 @@
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>10</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -9042,9 +9228,15 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="F35" s="1">
+        <v>5</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>9</v>
+      </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -9064,9 +9256,15 @@
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="F36" s="1">
+        <v>3</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2</v>
+      </c>
+      <c r="H36" s="1">
+        <v>25</v>
+      </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -9086,9 +9284,15 @@
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="F37" s="1">
+        <v>2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1">
+        <v>24</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -9108,9 +9312,15 @@
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>71</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -9130,9 +9340,15 @@
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>5</v>
+      </c>
+      <c r="H39" s="1">
+        <v>87</v>
+      </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -9152,9 +9368,15 @@
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="F40" s="1">
+        <v>4</v>
+      </c>
+      <c r="G40" s="1">
+        <v>5</v>
+      </c>
+      <c r="H40" s="1">
+        <v>65</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -9174,9 +9396,15 @@
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>51</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -9196,9 +9424,15 @@
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>15</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -9218,9 +9452,15 @@
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="F43" s="1">
+        <v>14</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
+        <v>7</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>

</xml_diff>